<commit_message>
autoit integration for test data
</commit_message>
<xml_diff>
--- a/Oragne_HRM_Advance/src/main/java/com/hrm/qa/testdata/TestData.xlsx
+++ b/Oragne_HRM_Advance/src/main/java/com/hrm/qa/testdata/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ramita Sambyal\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B19783DE-FB24-4487-A67B-9F7917D86299}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6414940-2071-467F-9172-3DB1B46F0D94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{8C30D4FD-073D-497C-8C0B-EDD7F3A02C26}"/>
+    <workbookView xWindow="2620" yWindow="2620" windowWidth="14400" windowHeight="8170" xr2:uid="{8C30D4FD-073D-497C-8C0B-EDD7F3A02C26}"/>
   </bookViews>
   <sheets>
     <sheet name="TestcasesData" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Name</t>
   </si>
@@ -70,6 +70,18 @@
   </si>
   <si>
     <t>anjali@yopmail.com</t>
+  </si>
+  <si>
+    <t>ResumeFilePath</t>
+  </si>
+  <si>
+    <t>C:\\Users\\Ramita Sambyal\\Desktop\\FileUploadAUTOIT.exe</t>
+  </si>
+  <si>
+    <t>C:\\Users\\Ramita Sambyal\\Desktop\\FileUploadAUTOITInvalidFormat.exe</t>
+  </si>
+  <si>
+    <t>C:\\Users\\Ramita Sambyal\\Desktop\\FileUploadAUTOITInvalidFormat2.exe</t>
   </si>
 </sst>
 </file>
@@ -432,18 +444,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2C9499D-6E95-4DC4-8C9A-3E75ED866080}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="25" customWidth="1"/>
+    <col min="4" max="4" width="63.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -453,8 +466,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -464,8 +480,11 @@
       <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -475,9 +494,12 @@
       <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
@@ -485,6 +507,9 @@
       </c>
       <c r="C4" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -492,6 +517,7 @@
     <hyperlink ref="C2" r:id="rId1" xr:uid="{BB2BE912-2D8F-4F58-8E32-EE7095EF4CDC}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{1BBC6C2D-BBB9-4ADB-B388-2B9CA47A6E9C}"/>
     <hyperlink ref="C4" r:id="rId3" xr:uid="{5CF2A4BA-A16D-4DA3-A853-E58F004153D9}"/>
+    <hyperlink ref="A4" r:id="rId4" display="anjali@" xr:uid="{F6F162E9-DE10-4FF5-9E18-A5F4BC359858}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>